<commit_message>
Add Evaluations of Interns
</commit_message>
<xml_diff>
--- a/Interns/Tracks of Interns.xlsx
+++ b/Interns/Tracks of Interns.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="21">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t xml:space="preserve">Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Careless, don’t what to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have ideas but should make more and further actions</t>
   </si>
   <si>
     <t xml:space="preserve">Tasks</t>
@@ -72,7 +81,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial Unicode MS"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -104,7 +113,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial Unicode MS"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -134,7 +143,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial Unicode MS"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -166,7 +175,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial Unicode MS"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -200,7 +209,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Arial Unicode MS"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -252,14 +261,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -323,24 +332,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +353,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,16 +361,32 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -445,23 +466,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3:J9"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.4489795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="26.3673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,7 +582,7 @@
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
     </row>
-    <row r="4" s="10" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -593,10 +613,8 @@
       <c r="J4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="0"/>
-      <c r="L4" s="0"/>
-    </row>
-    <row r="5" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,10 +645,8 @@
       <c r="J5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="0"/>
-      <c r="L5" s="0"/>
-    </row>
-    <row r="6" s="10" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -661,10 +677,8 @@
       <c r="J6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="0"/>
-      <c r="L6" s="0"/>
-    </row>
-    <row r="7" s="10" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -695,10 +709,8 @@
       <c r="J7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0"/>
-    </row>
-    <row r="8" s="10" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -729,81 +741,49 @@
       <c r="J8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0"/>
-    </row>
-    <row r="9" s="10" customFormat="true" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="D11" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="0"/>
-      <c r="L9" s="0"/>
-    </row>
-    <row r="10" s="10" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" s="10" customFormat="true" ht="59.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>0</v>
@@ -811,10 +791,68 @@
       <c r="F11" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>0</v>
+      <c r="G11" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="87.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -836,21 +874,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,标准"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,标准"Page &amp;P</oddFooter>
@@ -865,21 +902,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,标准"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,标准"Page &amp;P</oddFooter>

</xml_diff>